<commit_message>
startedÖBV-Ranglisten and finished spielerranglisten
</commit_message>
<xml_diff>
--- a/files/_development/spielerranglisten1718.xlsx
+++ b/files/_development/spielerranglisten1718.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Badminton\files\_development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002430F2-F9A8-438A-9D10-1969524BBC2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE2BDFF-A3CA-4B76-8B07-A1BD6846C6F8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4170" xr2:uid="{C72020F4-C860-4579-BD05-68AC76014F2D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="323">
   <si>
     <t>Nachname</t>
   </si>
@@ -633,6 +633,372 @@
   </si>
   <si>
     <t>David</t>
+  </si>
+  <si>
+    <t>Setina</t>
+  </si>
+  <si>
+    <t>Ana Marija</t>
+  </si>
+  <si>
+    <t>Langthaler</t>
+  </si>
+  <si>
+    <t>Sonja</t>
+  </si>
+  <si>
+    <t>Peshekhonova</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Kohlfürst(LS)</t>
+  </si>
+  <si>
+    <t>Sarina</t>
+  </si>
+  <si>
+    <t>Hofinger</t>
+  </si>
+  <si>
+    <t>Nader</t>
+  </si>
+  <si>
+    <t>Karina</t>
+  </si>
+  <si>
+    <t>Edelmüller</t>
+  </si>
+  <si>
+    <t>Ursula</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>Kosorus</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Perneder</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Poledna</t>
+  </si>
+  <si>
+    <t>Pia</t>
+  </si>
+  <si>
+    <t>ASKÖ BV Pasching</t>
+  </si>
+  <si>
+    <t>0676/81427620</t>
+  </si>
+  <si>
+    <t>Leisch</t>
+  </si>
+  <si>
+    <t>Dorn</t>
+  </si>
+  <si>
+    <t>Pröll</t>
+  </si>
+  <si>
+    <t>Karl</t>
+  </si>
+  <si>
+    <t>Kuri</t>
+  </si>
+  <si>
+    <t>Josef</t>
+  </si>
+  <si>
+    <t>Leidlmayer</t>
+  </si>
+  <si>
+    <t>Doris</t>
+  </si>
+  <si>
+    <t>Elisabeth</t>
+  </si>
+  <si>
+    <t>Schned</t>
+  </si>
+  <si>
+    <t>Ameseder</t>
+  </si>
+  <si>
+    <t>Karin</t>
+  </si>
+  <si>
+    <t>ASKÖ Traun</t>
+  </si>
+  <si>
+    <t>28.</t>
+  </si>
+  <si>
+    <t>29.</t>
+  </si>
+  <si>
+    <t>30.</t>
+  </si>
+  <si>
+    <t>31.</t>
+  </si>
+  <si>
+    <t>Grendt(LS)</t>
+  </si>
+  <si>
+    <t>Collins-Valentine</t>
+  </si>
+  <si>
+    <t>Filimon(EU)</t>
+  </si>
+  <si>
+    <t>Zauner</t>
+  </si>
+  <si>
+    <t>Serov</t>
+  </si>
+  <si>
+    <t>Ratzenböck</t>
+  </si>
+  <si>
+    <t>Ostermann</t>
+  </si>
+  <si>
+    <t>Jakob</t>
+  </si>
+  <si>
+    <t>Stündl</t>
+  </si>
+  <si>
+    <t>Froschauer</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Szöke(EU)</t>
+  </si>
+  <si>
+    <t>Gyula</t>
+  </si>
+  <si>
+    <t>Danninger</t>
+  </si>
+  <si>
+    <t>0664/4108801</t>
+  </si>
+  <si>
+    <t>0699/19211350</t>
+  </si>
+  <si>
+    <t>0650/6060210</t>
+  </si>
+  <si>
+    <t>Auberger</t>
+  </si>
+  <si>
+    <t>Otmar</t>
+  </si>
+  <si>
+    <t>Wieshofer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stockinger </t>
+  </si>
+  <si>
+    <t>Dietmar</t>
+  </si>
+  <si>
+    <t>Jannik</t>
+  </si>
+  <si>
+    <t>Holl</t>
+  </si>
+  <si>
+    <t>Gindelhumer</t>
+  </si>
+  <si>
+    <t>Buckstegen</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Giel</t>
+  </si>
+  <si>
+    <t>Michael Peter</t>
+  </si>
+  <si>
+    <t>Dirngrabner</t>
+  </si>
+  <si>
+    <t>Claus</t>
+  </si>
+  <si>
+    <t>Reifetshammer</t>
+  </si>
+  <si>
+    <t>Rudolf</t>
+  </si>
+  <si>
+    <t>Lösch</t>
+  </si>
+  <si>
+    <t>Dieter</t>
+  </si>
+  <si>
+    <t>Pospichal</t>
+  </si>
+  <si>
+    <t>Gustav Rudolf</t>
+  </si>
+  <si>
+    <t>Berndl</t>
+  </si>
+  <si>
+    <t>Spitzhofer</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Grum</t>
+  </si>
+  <si>
+    <t>Baumgartner</t>
+  </si>
+  <si>
+    <t>Herbert</t>
+  </si>
+  <si>
+    <t>Heidenreich (EU)</t>
+  </si>
+  <si>
+    <t>Lais (LS)</t>
+  </si>
+  <si>
+    <t>Janine</t>
+  </si>
+  <si>
+    <t>Zinganell</t>
+  </si>
+  <si>
+    <t>Lena</t>
+  </si>
+  <si>
+    <t>Hauser</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Scheer</t>
+  </si>
+  <si>
+    <t>Sendlhofer</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Lelaina</t>
+  </si>
+  <si>
+    <t>Reifetshamer</t>
+  </si>
+  <si>
+    <t>Karola</t>
+  </si>
+  <si>
+    <t>Pei</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Pohlmüller</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Weilguni</t>
+  </si>
+  <si>
+    <t>Bettina</t>
+  </si>
+  <si>
+    <t>Susanna</t>
+  </si>
+  <si>
+    <t>Zangenfeind</t>
+  </si>
+  <si>
+    <t>Katrin</t>
+  </si>
+  <si>
+    <t>Liga</t>
+  </si>
+  <si>
+    <t>Matric</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Stockinger</t>
+  </si>
+  <si>
+    <t>Lara</t>
+  </si>
+  <si>
+    <t>Fobian</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>Maibritt</t>
+  </si>
+  <si>
+    <t>Ronja</t>
+  </si>
+  <si>
+    <t>Dreu</t>
+  </si>
+  <si>
+    <t>Alina</t>
+  </si>
+  <si>
+    <t>Lanzerstorfer</t>
+  </si>
+  <si>
+    <t>Emma</t>
   </si>
 </sst>
 </file>
@@ -668,9 +1034,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,30 +1360,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E359FFB2-F4F7-45DC-A388-18C9B70D6F86}">
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G195" sqref="G195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1524,16 +1894,16 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1894,16 +2264,16 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
@@ -2384,16 +2754,16 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
@@ -2989,12 +3359,1701 @@
         <v>304</v>
       </c>
     </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
+        <v>202</v>
+      </c>
+      <c r="D108">
+        <v>36733</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109">
+        <v>20980</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
+        <v>207</v>
+      </c>
+      <c r="D110">
+        <v>70634</v>
+      </c>
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="F110">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>10</v>
+      </c>
+      <c r="B111" t="s">
+        <v>208</v>
+      </c>
+      <c r="C111" t="s">
+        <v>209</v>
+      </c>
+      <c r="D111">
+        <v>61359</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>11</v>
+      </c>
+      <c r="B112" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" t="s">
+        <v>206</v>
+      </c>
+      <c r="D112">
+        <v>31522</v>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" t="s">
+        <v>211</v>
+      </c>
+      <c r="C113" t="s">
+        <v>212</v>
+      </c>
+      <c r="D113">
+        <v>30038</v>
+      </c>
+      <c r="E113">
+        <v>3</v>
+      </c>
+      <c r="F113">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" t="s">
+        <v>213</v>
+      </c>
+      <c r="C114" t="s">
+        <v>214</v>
+      </c>
+      <c r="D114">
+        <v>3172</v>
+      </c>
+      <c r="E114">
+        <v>3</v>
+      </c>
+      <c r="F114">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115" t="s">
+        <v>215</v>
+      </c>
+      <c r="C115" t="s">
+        <v>216</v>
+      </c>
+      <c r="D115">
+        <v>10768</v>
+      </c>
+      <c r="E115">
+        <v>3</v>
+      </c>
+      <c r="F115">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" t="s">
+        <v>191</v>
+      </c>
+      <c r="C116" t="s">
+        <v>51</v>
+      </c>
+      <c r="D116">
+        <v>32455</v>
+      </c>
+      <c r="E116">
+        <v>3</v>
+      </c>
+      <c r="F116">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" t="s">
+        <v>217</v>
+      </c>
+      <c r="C117" t="s">
+        <v>218</v>
+      </c>
+      <c r="D117">
+        <v>34773</v>
+      </c>
+      <c r="E117">
+        <v>3</v>
+      </c>
+      <c r="F117">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" t="s">
+        <v>219</v>
+      </c>
+      <c r="C118" t="s">
+        <v>220</v>
+      </c>
+      <c r="D118">
+        <v>34157</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+      <c r="F118">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119" t="s">
+        <v>194</v>
+      </c>
+      <c r="C119" t="s">
+        <v>221</v>
+      </c>
+      <c r="D119">
+        <v>36697</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+      <c r="F119">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120" t="s">
+        <v>222</v>
+      </c>
+      <c r="C120" t="s">
+        <v>223</v>
+      </c>
+      <c r="D120">
+        <v>38434</v>
+      </c>
+      <c r="E120">
+        <v>3</v>
+      </c>
+      <c r="F120">
+        <v>304</v>
+      </c>
+      <c r="G120" s="1">
+        <v>43086</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>2</v>
+      </c>
+      <c r="E124" t="s">
+        <v>3</v>
+      </c>
+      <c r="F124" t="s">
+        <v>4</v>
+      </c>
+      <c r="G124" t="s">
+        <v>60</v>
+      </c>
+      <c r="H124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" t="s">
+        <v>226</v>
+      </c>
+      <c r="C125" t="s">
+        <v>34</v>
+      </c>
+      <c r="D125">
+        <v>30921</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" t="s">
+        <v>226</v>
+      </c>
+      <c r="C126" t="s">
+        <v>165</v>
+      </c>
+      <c r="D126">
+        <v>31988</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" t="s">
+        <v>227</v>
+      </c>
+      <c r="C127" t="s">
+        <v>111</v>
+      </c>
+      <c r="D127">
+        <v>1275</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>10</v>
+      </c>
+      <c r="B128" t="s">
+        <v>226</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
+      </c>
+      <c r="D128">
+        <v>1272</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" t="s">
+        <v>228</v>
+      </c>
+      <c r="C129" t="s">
+        <v>229</v>
+      </c>
+      <c r="D129">
+        <v>1275</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>305</v>
+      </c>
+      <c r="G129" t="s">
+        <v>77</v>
+      </c>
+      <c r="H129" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" t="s">
+        <v>230</v>
+      </c>
+      <c r="C130" t="s">
+        <v>231</v>
+      </c>
+      <c r="D130">
+        <v>1270</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>13</v>
+      </c>
+      <c r="B131" t="s">
+        <v>227</v>
+      </c>
+      <c r="C131" t="s">
+        <v>200</v>
+      </c>
+      <c r="D131">
+        <v>32372</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" t="s">
+        <v>232</v>
+      </c>
+      <c r="C133" t="s">
+        <v>233</v>
+      </c>
+      <c r="D133">
+        <v>30504</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" t="s">
+        <v>228</v>
+      </c>
+      <c r="C134" t="s">
+        <v>234</v>
+      </c>
+      <c r="D134">
+        <v>1274</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135" t="s">
+        <v>235</v>
+      </c>
+      <c r="C135" t="s">
+        <v>54</v>
+      </c>
+      <c r="D135">
+        <v>30505</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" t="s">
+        <v>236</v>
+      </c>
+      <c r="C136" t="s">
+        <v>237</v>
+      </c>
+      <c r="D136">
+        <v>35253</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D140" t="s">
+        <v>2</v>
+      </c>
+      <c r="E140" t="s">
+        <v>3</v>
+      </c>
+      <c r="F140" t="s">
+        <v>4</v>
+      </c>
+      <c r="G140" t="s">
+        <v>60</v>
+      </c>
+      <c r="H140" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>7</v>
+      </c>
+      <c r="B141" t="s">
+        <v>243</v>
+      </c>
+      <c r="C141" t="s">
+        <v>153</v>
+      </c>
+      <c r="D141">
+        <v>21139</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>72</v>
+      </c>
+      <c r="C142" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142">
+        <v>1313</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>9</v>
+      </c>
+      <c r="B143" t="s">
+        <v>245</v>
+      </c>
+      <c r="C143" t="s">
+        <v>244</v>
+      </c>
+      <c r="D143">
+        <v>37394</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>10</v>
+      </c>
+      <c r="B144" t="s">
+        <v>246</v>
+      </c>
+      <c r="C144" t="s">
+        <v>69</v>
+      </c>
+      <c r="D144">
+        <v>1749</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>11</v>
+      </c>
+      <c r="B145" t="s">
+        <v>247</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145">
+        <v>31894</v>
+      </c>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>248</v>
+      </c>
+      <c r="C146" t="s">
+        <v>26</v>
+      </c>
+      <c r="D146">
+        <v>30640</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" t="s">
+        <v>249</v>
+      </c>
+      <c r="C147" t="s">
+        <v>250</v>
+      </c>
+      <c r="D147">
+        <v>31874</v>
+      </c>
+      <c r="E147">
+        <v>2</v>
+      </c>
+      <c r="F147">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>14</v>
+      </c>
+      <c r="B148" t="s">
+        <v>251</v>
+      </c>
+      <c r="C148" t="s">
+        <v>111</v>
+      </c>
+      <c r="D148">
+        <v>1326</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
+      </c>
+      <c r="F148">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>15</v>
+      </c>
+      <c r="B149" t="s">
+        <v>72</v>
+      </c>
+      <c r="C149" t="s">
+        <v>163</v>
+      </c>
+      <c r="D149">
+        <v>1311</v>
+      </c>
+      <c r="E149">
+        <v>3</v>
+      </c>
+      <c r="F149">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>16</v>
+      </c>
+      <c r="B150" t="s">
+        <v>252</v>
+      </c>
+      <c r="C150" t="s">
+        <v>253</v>
+      </c>
+      <c r="D150">
+        <v>34973</v>
+      </c>
+      <c r="E150">
+        <v>3</v>
+      </c>
+      <c r="F150">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>17</v>
+      </c>
+      <c r="B151" t="s">
+        <v>254</v>
+      </c>
+      <c r="C151" t="s">
+        <v>255</v>
+      </c>
+      <c r="D151">
+        <v>38114</v>
+      </c>
+      <c r="E151">
+        <v>3</v>
+      </c>
+      <c r="F151">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>18</v>
+      </c>
+      <c r="B152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C152" t="s">
+        <v>163</v>
+      </c>
+      <c r="D152">
+        <v>31709</v>
+      </c>
+      <c r="E152">
+        <v>3</v>
+      </c>
+      <c r="F152">
+        <v>307</v>
+      </c>
+      <c r="G152" t="s">
+        <v>63</v>
+      </c>
+      <c r="H152" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>19</v>
+      </c>
+      <c r="B153" t="s">
+        <v>260</v>
+      </c>
+      <c r="C153" t="s">
+        <v>261</v>
+      </c>
+      <c r="D153">
+        <v>3420</v>
+      </c>
+      <c r="E153">
+        <v>4</v>
+      </c>
+      <c r="F153">
+        <v>307</v>
+      </c>
+      <c r="G153" t="s">
+        <v>178</v>
+      </c>
+      <c r="H153" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>20</v>
+      </c>
+      <c r="B154" t="s">
+        <v>263</v>
+      </c>
+      <c r="C154" t="s">
+        <v>264</v>
+      </c>
+      <c r="D154">
+        <v>35193</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+      <c r="F154">
+        <v>307</v>
+      </c>
+      <c r="G154" t="s">
+        <v>192</v>
+      </c>
+      <c r="H154" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>97</v>
+      </c>
+      <c r="B155" t="s">
+        <v>260</v>
+      </c>
+      <c r="C155" t="s">
+        <v>265</v>
+      </c>
+      <c r="D155">
+        <v>35215</v>
+      </c>
+      <c r="E155">
+        <v>4</v>
+      </c>
+      <c r="F155">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>140</v>
+      </c>
+      <c r="B156" t="s">
+        <v>262</v>
+      </c>
+      <c r="C156" t="s">
+        <v>122</v>
+      </c>
+      <c r="D156">
+        <v>31639</v>
+      </c>
+      <c r="E156">
+        <v>4</v>
+      </c>
+      <c r="F156">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>141</v>
+      </c>
+      <c r="B157" t="s">
+        <v>252</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157">
+        <v>35174</v>
+      </c>
+      <c r="E157">
+        <v>4</v>
+      </c>
+      <c r="F157">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>142</v>
+      </c>
+      <c r="B158" t="s">
+        <v>266</v>
+      </c>
+      <c r="C158" t="s">
+        <v>42</v>
+      </c>
+      <c r="D158">
+        <v>32507</v>
+      </c>
+      <c r="E158">
+        <v>4</v>
+      </c>
+      <c r="F158">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>143</v>
+      </c>
+      <c r="B159" t="s">
+        <v>267</v>
+      </c>
+      <c r="C159" t="s">
+        <v>169</v>
+      </c>
+      <c r="D159">
+        <v>31195</v>
+      </c>
+      <c r="E159">
+        <v>4</v>
+      </c>
+      <c r="F159">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>144</v>
+      </c>
+      <c r="B160" t="s">
+        <v>268</v>
+      </c>
+      <c r="C160" t="s">
+        <v>269</v>
+      </c>
+      <c r="D160">
+        <v>35654</v>
+      </c>
+      <c r="E160">
+        <v>4</v>
+      </c>
+      <c r="F160">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>145</v>
+      </c>
+      <c r="B161" t="s">
+        <v>270</v>
+      </c>
+      <c r="C161" t="s">
+        <v>271</v>
+      </c>
+      <c r="D161">
+        <v>31310</v>
+      </c>
+      <c r="E161">
+        <v>4</v>
+      </c>
+      <c r="F161">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>146</v>
+      </c>
+      <c r="B162" t="s">
+        <v>274</v>
+      </c>
+      <c r="C162" t="s">
+        <v>275</v>
+      </c>
+      <c r="D162">
+        <v>31191</v>
+      </c>
+      <c r="E162">
+        <v>4</v>
+      </c>
+      <c r="F162">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>147</v>
+      </c>
+      <c r="B163" t="s">
+        <v>272</v>
+      </c>
+      <c r="C163" t="s">
+        <v>273</v>
+      </c>
+      <c r="D163">
+        <v>1713</v>
+      </c>
+      <c r="E163">
+        <v>4</v>
+      </c>
+      <c r="F163">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>148</v>
+      </c>
+      <c r="B164" t="s">
+        <v>276</v>
+      </c>
+      <c r="C164" t="s">
+        <v>277</v>
+      </c>
+      <c r="D164">
+        <v>31080</v>
+      </c>
+      <c r="E164">
+        <v>4</v>
+      </c>
+      <c r="F164">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>149</v>
+      </c>
+      <c r="B165" t="s">
+        <v>278</v>
+      </c>
+      <c r="C165" t="s">
+        <v>279</v>
+      </c>
+      <c r="D165">
+        <v>32600</v>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+      <c r="F165">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>150</v>
+      </c>
+      <c r="B166" t="s">
+        <v>280</v>
+      </c>
+      <c r="C166" t="s">
+        <v>231</v>
+      </c>
+      <c r="D166">
+        <v>32634</v>
+      </c>
+      <c r="E166">
+        <v>4</v>
+      </c>
+      <c r="F166">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>151</v>
+      </c>
+      <c r="B167" t="s">
+        <v>281</v>
+      </c>
+      <c r="C167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D167">
+        <v>37177</v>
+      </c>
+      <c r="E167">
+        <v>4</v>
+      </c>
+      <c r="F167">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>239</v>
+      </c>
+      <c r="B168" t="s">
+        <v>263</v>
+      </c>
+      <c r="C168" t="s">
+        <v>283</v>
+      </c>
+      <c r="D168">
+        <v>35214</v>
+      </c>
+      <c r="E168">
+        <v>4</v>
+      </c>
+      <c r="F168">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>240</v>
+      </c>
+      <c r="B169" t="s">
+        <v>284</v>
+      </c>
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169">
+        <v>37433</v>
+      </c>
+      <c r="E169">
+        <v>4</v>
+      </c>
+      <c r="F169">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>241</v>
+      </c>
+      <c r="B170" t="s">
+        <v>285</v>
+      </c>
+      <c r="C170" t="s">
+        <v>99</v>
+      </c>
+      <c r="D170">
+        <v>37174</v>
+      </c>
+      <c r="E170">
+        <v>4</v>
+      </c>
+      <c r="F170">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>242</v>
+      </c>
+      <c r="B171" t="s">
+        <v>72</v>
+      </c>
+      <c r="C171" t="s">
+        <v>286</v>
+      </c>
+      <c r="D171">
+        <v>1312</v>
+      </c>
+      <c r="E171">
+        <v>4</v>
+      </c>
+      <c r="F171">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>7</v>
+      </c>
+      <c r="B173" t="s">
+        <v>287</v>
+      </c>
+      <c r="C173" t="s">
+        <v>221</v>
+      </c>
+      <c r="D173">
+        <v>38113</v>
+      </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174" t="s">
+        <v>288</v>
+      </c>
+      <c r="C174" t="s">
+        <v>289</v>
+      </c>
+      <c r="D174">
+        <v>61722</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>9</v>
+      </c>
+      <c r="B175" t="s">
+        <v>290</v>
+      </c>
+      <c r="C175" t="s">
+        <v>291</v>
+      </c>
+      <c r="D175">
+        <v>32409</v>
+      </c>
+      <c r="E175">
+        <v>2</v>
+      </c>
+      <c r="F175">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176" t="s">
+        <v>292</v>
+      </c>
+      <c r="C176" t="s">
+        <v>293</v>
+      </c>
+      <c r="D176">
+        <v>32243</v>
+      </c>
+      <c r="E176">
+        <v>2</v>
+      </c>
+      <c r="F176">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>11</v>
+      </c>
+      <c r="B177" t="s">
+        <v>294</v>
+      </c>
+      <c r="C177" t="s">
+        <v>129</v>
+      </c>
+      <c r="D177">
+        <v>31044</v>
+      </c>
+      <c r="E177">
+        <v>3</v>
+      </c>
+      <c r="F177">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>12</v>
+      </c>
+      <c r="B178" t="s">
+        <v>295</v>
+      </c>
+      <c r="C178" t="s">
+        <v>296</v>
+      </c>
+      <c r="D178">
+        <v>32168</v>
+      </c>
+      <c r="E178">
+        <v>3</v>
+      </c>
+      <c r="F178">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B179" t="s">
+        <v>297</v>
+      </c>
+      <c r="C179" t="s">
+        <v>298</v>
+      </c>
+      <c r="D179">
+        <v>32146</v>
+      </c>
+      <c r="E179">
+        <v>4</v>
+      </c>
+      <c r="F179">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>14</v>
+      </c>
+      <c r="B180" t="s">
+        <v>299</v>
+      </c>
+      <c r="C180" t="s">
+        <v>300</v>
+      </c>
+      <c r="D180">
+        <v>31362</v>
+      </c>
+      <c r="E180">
+        <v>4</v>
+      </c>
+      <c r="F180">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>15</v>
+      </c>
+      <c r="B181" t="s">
+        <v>301</v>
+      </c>
+      <c r="C181" t="s">
+        <v>302</v>
+      </c>
+      <c r="D181">
+        <v>3852</v>
+      </c>
+      <c r="E181">
+        <v>4</v>
+      </c>
+      <c r="F181">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>16</v>
+      </c>
+      <c r="B182" t="s">
+        <v>303</v>
+      </c>
+      <c r="C182" t="s">
+        <v>304</v>
+      </c>
+      <c r="D182">
+        <v>31573</v>
+      </c>
+      <c r="E182">
+        <v>4</v>
+      </c>
+      <c r="F182">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>17</v>
+      </c>
+      <c r="B183" t="s">
+        <v>305</v>
+      </c>
+      <c r="C183" t="s">
+        <v>306</v>
+      </c>
+      <c r="D183">
+        <v>1179</v>
+      </c>
+      <c r="E183">
+        <v>4</v>
+      </c>
+      <c r="F183">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>18</v>
+      </c>
+      <c r="B184" t="s">
+        <v>260</v>
+      </c>
+      <c r="C184" t="s">
+        <v>307</v>
+      </c>
+      <c r="D184">
+        <v>35373</v>
+      </c>
+      <c r="E184">
+        <v>4</v>
+      </c>
+      <c r="F184">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>19</v>
+      </c>
+      <c r="B185" t="s">
+        <v>281</v>
+      </c>
+      <c r="C185" t="s">
+        <v>54</v>
+      </c>
+      <c r="D185">
+        <v>37253</v>
+      </c>
+      <c r="E185">
+        <v>4</v>
+      </c>
+      <c r="F185">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>20</v>
+      </c>
+      <c r="B186" t="s">
+        <v>284</v>
+      </c>
+      <c r="C186" t="s">
+        <v>306</v>
+      </c>
+      <c r="D186">
+        <v>37393</v>
+      </c>
+      <c r="E186">
+        <v>4</v>
+      </c>
+      <c r="F186">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>97</v>
+      </c>
+      <c r="B187" t="s">
+        <v>308</v>
+      </c>
+      <c r="C187" t="s">
+        <v>309</v>
+      </c>
+      <c r="D187">
+        <v>35873</v>
+      </c>
+      <c r="E187">
+        <v>4</v>
+      </c>
+      <c r="F187">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>140</v>
+      </c>
+      <c r="B188" t="s">
+        <v>248</v>
+      </c>
+      <c r="C188" t="s">
+        <v>310</v>
+      </c>
+      <c r="D188">
+        <v>36913</v>
+      </c>
+      <c r="E188">
+        <v>4</v>
+      </c>
+      <c r="F188">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>141</v>
+      </c>
+      <c r="B189" t="s">
+        <v>311</v>
+      </c>
+      <c r="C189" t="s">
+        <v>312</v>
+      </c>
+      <c r="D189">
+        <v>36373</v>
+      </c>
+      <c r="E189">
+        <v>4</v>
+      </c>
+      <c r="F189">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>142</v>
+      </c>
+      <c r="B190" t="s">
+        <v>313</v>
+      </c>
+      <c r="C190" t="s">
+        <v>314</v>
+      </c>
+      <c r="D190">
+        <v>35213</v>
+      </c>
+      <c r="E190">
+        <v>4</v>
+      </c>
+      <c r="F190">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>143</v>
+      </c>
+      <c r="B191" t="s">
+        <v>315</v>
+      </c>
+      <c r="C191" t="s">
+        <v>316</v>
+      </c>
+      <c r="D191">
+        <v>36914</v>
+      </c>
+      <c r="E191">
+        <v>4</v>
+      </c>
+      <c r="F191">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>144</v>
+      </c>
+      <c r="B192" t="s">
+        <v>315</v>
+      </c>
+      <c r="C192" t="s">
+        <v>317</v>
+      </c>
+      <c r="D192">
+        <v>36014</v>
+      </c>
+      <c r="E192">
+        <v>4</v>
+      </c>
+      <c r="F192">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>145</v>
+      </c>
+      <c r="B193" t="s">
+        <v>260</v>
+      </c>
+      <c r="C193" t="s">
+        <v>318</v>
+      </c>
+      <c r="D193">
+        <v>36013</v>
+      </c>
+      <c r="E193">
+        <v>4</v>
+      </c>
+      <c r="F193">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>146</v>
+      </c>
+      <c r="B194" t="s">
+        <v>319</v>
+      </c>
+      <c r="C194" t="s">
+        <v>312</v>
+      </c>
+      <c r="D194">
+        <v>37176</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+      <c r="F194">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>147</v>
+      </c>
+      <c r="B195" t="s">
+        <v>285</v>
+      </c>
+      <c r="C195" t="s">
+        <v>320</v>
+      </c>
+      <c r="D195">
+        <v>37175</v>
+      </c>
+      <c r="E195">
+        <v>4</v>
+      </c>
+      <c r="F195">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>148</v>
+      </c>
+      <c r="B196" t="s">
+        <v>321</v>
+      </c>
+      <c r="C196" t="s">
+        <v>322</v>
+      </c>
+      <c r="D196">
+        <v>37173</v>
+      </c>
+      <c r="E196">
+        <v>4</v>
+      </c>
+      <c r="F196">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A138:H138"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="A50:H50"/>
     <mergeCell ref="A77:H77"/>
+    <mergeCell ref="A122:H122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>